<commit_message>
add html & twdx files
</commit_message>
<xml_diff>
--- a/Interview Table(SQL).xlsx
+++ b/Interview Table(SQL).xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24302"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jw5830\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D993AEE-785E-4434-B931-50B480254AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{6D993AEE-785E-4434-B931-50B480254AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA8B0A0A-35EA-4CD7-BF28-8707F8D7A849}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{966433DB-B6F8-447F-9314-2AB34DA0283B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{966433DB-B6F8-447F-9314-2AB34DA0283B}"/>
   </bookViews>
   <sheets>
     <sheet name="CaseTable" sheetId="1" r:id="rId1"/>
-    <sheet name="Provider Table" sheetId="2" r:id="rId2"/>
-    <sheet name="Member Table" sheetId="3" r:id="rId3"/>
+    <sheet name="ProviderTable" sheetId="2" r:id="rId2"/>
+    <sheet name="MemberTable" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -46,235 +47,235 @@
     <t>Date</t>
   </si>
   <si>
+    <t>DischargeDate</t>
+  </si>
+  <si>
     <t>CaseNumber</t>
   </si>
   <si>
     <t>Diag</t>
   </si>
   <si>
+    <t>K70</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>I44</t>
+  </si>
+  <si>
+    <t>E66</t>
+  </si>
+  <si>
+    <t>N81</t>
+  </si>
+  <si>
+    <t>F32</t>
+  </si>
+  <si>
+    <t>I34</t>
+  </si>
+  <si>
+    <t>K80</t>
+  </si>
+  <si>
+    <t>G50</t>
+  </si>
+  <si>
+    <t>F40</t>
+  </si>
+  <si>
+    <t>D50</t>
+  </si>
+  <si>
+    <t>N20</t>
+  </si>
+  <si>
+    <t>N39.3</t>
+  </si>
+  <si>
+    <t>M05</t>
+  </si>
+  <si>
+    <t>K57</t>
+  </si>
+  <si>
+    <t>F45</t>
+  </si>
+  <si>
+    <t>H90</t>
+  </si>
+  <si>
+    <t>I60</t>
+  </si>
+  <si>
+    <t>I5O</t>
+  </si>
+  <si>
+    <t>J40</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>I10</t>
+  </si>
+  <si>
     <t>AdmitDate</t>
   </si>
   <si>
     <t>Provider</t>
   </si>
   <si>
+    <t>563732370</t>
+  </si>
+  <si>
+    <t>Mt Carmel Grove City</t>
+  </si>
+  <si>
+    <t>Mt Carmel Hilliard</t>
+  </si>
+  <si>
+    <t>Mt Carmel New Albany</t>
+  </si>
+  <si>
+    <t>563732371</t>
+  </si>
+  <si>
+    <t>Osu - University Hospital East</t>
+  </si>
+  <si>
+    <t>6493453930</t>
+  </si>
+  <si>
+    <t>OTHER UNION</t>
+  </si>
+  <si>
+    <t>7492474291</t>
+  </si>
+  <si>
+    <t>OHIO HEALTH</t>
+  </si>
+  <si>
+    <t>CRYSTAL CLINIC ORTHOPAEDIC CTR</t>
+  </si>
+  <si>
+    <t>OTHER SUMMIT</t>
+  </si>
+  <si>
+    <t>UNIV HOSPITALS</t>
+  </si>
+  <si>
+    <t>OTHER TUSCARAWAS</t>
+  </si>
+  <si>
+    <t>3362848470</t>
+  </si>
+  <si>
+    <t>Metrohealth Medical Ctr</t>
+  </si>
+  <si>
+    <t>4734634290</t>
+  </si>
+  <si>
+    <t>3349474250</t>
+  </si>
+  <si>
+    <t>3848346481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">St Elizabeth </t>
+  </si>
+  <si>
+    <t>4034886281</t>
+  </si>
+  <si>
+    <t>4828646420</t>
+  </si>
+  <si>
+    <t>Bucyrus Community Hospital</t>
+  </si>
+  <si>
+    <t>5738504641</t>
+  </si>
+  <si>
+    <t>East Liverpool City Hospital</t>
+  </si>
+  <si>
+    <t>5355385781</t>
+  </si>
+  <si>
+    <t>Ohio Valley Surgical Hospital</t>
+  </si>
+  <si>
+    <t>8463645330</t>
+  </si>
+  <si>
+    <t>Mercy Health – Fairfield Hospital</t>
+  </si>
+  <si>
+    <t>Hamilton Va Cboc</t>
+  </si>
+  <si>
+    <t>Uc Health West Chester Hospital</t>
+  </si>
+  <si>
+    <t>Fort Hamilton Hospital</t>
+  </si>
+  <si>
+    <t>3757368630</t>
+  </si>
+  <si>
+    <t>Belmont Community Hospital</t>
+  </si>
+  <si>
+    <t>3757368631</t>
+  </si>
+  <si>
+    <t>8483646651</t>
+  </si>
+  <si>
+    <t>Galion Community Hosp</t>
+  </si>
+  <si>
+    <t>3849385041</t>
+  </si>
+  <si>
+    <t>Ohiohealth Grant Medical Center</t>
+  </si>
+  <si>
+    <t>Osu - University Hospital Wexner</t>
+  </si>
+  <si>
+    <t>9374973660</t>
+  </si>
+  <si>
+    <t>8374593960</t>
+  </si>
+  <si>
+    <t>Ohiohealth Grove City Methodist Hospital</t>
+  </si>
+  <si>
+    <t>5869040551</t>
+  </si>
+  <si>
+    <t>Uh Cleveland Medical Center</t>
+  </si>
+  <si>
+    <t>3894959301</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>563732370</t>
-  </si>
-  <si>
-    <t>563732371</t>
-  </si>
-  <si>
-    <t>6493453930</t>
-  </si>
-  <si>
-    <t>7492474291</t>
-  </si>
-  <si>
-    <t>3362848470</t>
-  </si>
-  <si>
-    <t>4734634290</t>
-  </si>
-  <si>
-    <t>3349474250</t>
-  </si>
-  <si>
-    <t>3848346481</t>
-  </si>
-  <si>
-    <t>4034886281</t>
-  </si>
-  <si>
-    <t>4828646420</t>
-  </si>
-  <si>
-    <t>5738504641</t>
-  </si>
-  <si>
-    <t>5355385781</t>
-  </si>
-  <si>
-    <t>8463645330</t>
-  </si>
-  <si>
-    <t>3757368630</t>
-  </si>
-  <si>
-    <t>3757368631</t>
-  </si>
-  <si>
-    <t>8483646651</t>
-  </si>
-  <si>
-    <t>3849385041</t>
-  </si>
-  <si>
-    <t>9374973660</t>
-  </si>
-  <si>
-    <t>8374593960</t>
-  </si>
-  <si>
-    <t>5869040551</t>
-  </si>
-  <si>
-    <t>3894959301</t>
-  </si>
-  <si>
-    <t>Mt Carmel Grove City</t>
-  </si>
-  <si>
-    <t>Mt Carmel Hilliard</t>
-  </si>
-  <si>
-    <t>Mt Carmel New Albany</t>
-  </si>
-  <si>
-    <t>Osu - University Hospital East</t>
-  </si>
-  <si>
-    <t>OTHER UNION</t>
-  </si>
-  <si>
-    <t>OHIO HEALTH</t>
-  </si>
-  <si>
-    <t>CRYSTAL CLINIC ORTHOPAEDIC CTR</t>
-  </si>
-  <si>
-    <t>OTHER SUMMIT</t>
-  </si>
-  <si>
-    <t>UNIV HOSPITALS</t>
-  </si>
-  <si>
-    <t>OTHER TUSCARAWAS</t>
-  </si>
-  <si>
-    <t>Metrohealth Medical Ctr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St Elizabeth </t>
-  </si>
-  <si>
-    <t>Bucyrus Community Hospital</t>
-  </si>
-  <si>
-    <t>East Liverpool City Hospital</t>
-  </si>
-  <si>
-    <t>Ohio Valley Surgical Hospital</t>
-  </si>
-  <si>
-    <t>Mercy Health – Fairfield Hospital</t>
-  </si>
-  <si>
-    <t>Hamilton Va Cboc</t>
-  </si>
-  <si>
-    <t>Uc Health West Chester Hospital</t>
-  </si>
-  <si>
-    <t>Fort Hamilton Hospital</t>
-  </si>
-  <si>
-    <t>Belmont Community Hospital</t>
-  </si>
-  <si>
-    <t>Galion Community Hosp</t>
-  </si>
-  <si>
-    <t>Ohiohealth Grant Medical Center</t>
-  </si>
-  <si>
-    <t>Osu - University Hospital Wexner</t>
-  </si>
-  <si>
-    <t>Ohiohealth Grove City Methodist Hospital</t>
-  </si>
-  <si>
-    <t>Uh Cleveland Medical Center</t>
+    <t>DateOfBirth</t>
   </si>
   <si>
     <t>M</t>
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>DateOfBirth</t>
-  </si>
-  <si>
-    <t>K70</t>
-  </si>
-  <si>
-    <t>F32</t>
-  </si>
-  <si>
-    <t>E10</t>
-  </si>
-  <si>
-    <t>I44</t>
-  </si>
-  <si>
-    <t>E66</t>
-  </si>
-  <si>
-    <t>N81</t>
-  </si>
-  <si>
-    <t>K80</t>
-  </si>
-  <si>
-    <t>I34</t>
-  </si>
-  <si>
-    <t>G50</t>
-  </si>
-  <si>
-    <t>F40</t>
-  </si>
-  <si>
-    <t>D50</t>
-  </si>
-  <si>
-    <t>N20</t>
-  </si>
-  <si>
-    <t>N39.3</t>
-  </si>
-  <si>
-    <t>M05</t>
-  </si>
-  <si>
-    <t>K57</t>
-  </si>
-  <si>
-    <t>F45</t>
-  </si>
-  <si>
-    <t>H90</t>
-  </si>
-  <si>
-    <t>I60</t>
-  </si>
-  <si>
-    <t>I5O</t>
-  </si>
-  <si>
-    <t>J40</t>
-  </si>
-  <si>
-    <t>E01</t>
-  </si>
-  <si>
-    <t>I10</t>
-  </si>
-  <si>
-    <t>DischargeDate</t>
   </si>
 </sst>
 </file>
@@ -285,7 +286,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,20 +636,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF4C409-F0D9-456F-A14D-5E3EAF3898A5}">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -659,16 +660,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>56373237</v>
       </c>
@@ -685,10 +686,10 @@
         <v>21678</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>56373237</v>
       </c>
@@ -705,10 +706,10 @@
         <v>73643</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>56373237</v>
       </c>
@@ -725,10 +726,10 @@
         <v>39493</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>56373237</v>
       </c>
@@ -745,10 +746,10 @@
         <v>90384</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>56373237</v>
       </c>
@@ -765,10 +766,10 @@
         <v>23947</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>56373237</v>
       </c>
@@ -785,10 +786,10 @@
         <v>27429</v>
       </c>
       <c r="F7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>649345393</v>
       </c>
@@ -805,10 +806,10 @@
         <v>42477</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>649345393</v>
       </c>
@@ -825,10 +826,10 @@
         <v>23394</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>649345393</v>
       </c>
@@ -845,10 +846,10 @@
         <v>29404</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>649345393</v>
       </c>
@@ -865,10 +866,10 @@
         <v>49249</v>
       </c>
       <c r="F11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>649345393</v>
       </c>
@@ -885,10 +886,10 @@
         <v>94029</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>749247429</v>
       </c>
@@ -905,10 +906,10 @@
         <v>94944</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>749247429</v>
       </c>
@@ -925,10 +926,10 @@
         <v>93948</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>749247429</v>
       </c>
@@ -945,10 +946,10 @@
         <v>23949</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>749247429</v>
       </c>
@@ -965,10 +966,10 @@
         <v>20420</v>
       </c>
       <c r="F16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>749247429</v>
       </c>
@@ -985,10 +986,10 @@
         <v>85020</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>336284847</v>
       </c>
@@ -1005,10 +1006,10 @@
         <v>12739</v>
       </c>
       <c r="F18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>473463429</v>
       </c>
@@ -1025,10 +1026,10 @@
         <v>53432</v>
       </c>
       <c r="F19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>334947425</v>
       </c>
@@ -1045,10 +1046,10 @@
         <v>28098</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>334947425</v>
       </c>
@@ -1065,10 +1066,10 @@
         <v>40478</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>334947425</v>
       </c>
@@ -1085,10 +1086,10 @@
         <v>36170</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>384834648</v>
       </c>
@@ -1105,10 +1106,10 @@
         <v>83281</v>
       </c>
       <c r="F23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>403488628</v>
       </c>
@@ -1125,10 +1126,10 @@
         <v>39366</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>403488628</v>
       </c>
@@ -1145,10 +1146,10 @@
         <v>38129</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>403488628</v>
       </c>
@@ -1165,10 +1166,10 @@
         <v>60489</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>482864642</v>
       </c>
@@ -1185,10 +1186,10 @@
         <v>59410</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>573850464</v>
       </c>
@@ -1205,10 +1206,10 @@
         <v>60228</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>535538578</v>
       </c>
@@ -1225,10 +1226,10 @@
         <v>74420</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>846364533</v>
       </c>
@@ -1245,10 +1246,10 @@
         <v>30861</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>846364533</v>
       </c>
@@ -1265,10 +1266,10 @@
         <v>49212</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>846364533</v>
       </c>
@@ -1285,10 +1286,10 @@
         <v>59226</v>
       </c>
       <c r="F32" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>846364533</v>
       </c>
@@ -1305,10 +1306,10 @@
         <v>27915</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>846364533</v>
       </c>
@@ -1325,10 +1326,10 @@
         <v>66470</v>
       </c>
       <c r="F34" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>375736863</v>
       </c>
@@ -1345,10 +1346,10 @@
         <v>54771</v>
       </c>
       <c r="F35" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>375736863</v>
       </c>
@@ -1365,10 +1366,10 @@
         <v>33046</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>848364665</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>73447</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>384938504</v>
       </c>
@@ -1402,10 +1403,10 @@
         <v>82199</v>
       </c>
       <c r="F38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>384938504</v>
       </c>
@@ -1422,10 +1423,10 @@
         <v>46278</v>
       </c>
       <c r="F39" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>937497366</v>
       </c>
@@ -1442,10 +1443,10 @@
         <v>76213</v>
       </c>
       <c r="F40" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>837459396</v>
       </c>
@@ -1462,10 +1463,10 @@
         <v>28621</v>
       </c>
       <c r="F41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>837459396</v>
       </c>
@@ -1482,10 +1483,10 @@
         <v>59757</v>
       </c>
       <c r="F42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>586904055</v>
       </c>
@@ -1502,10 +1503,10 @@
         <v>38699</v>
       </c>
       <c r="F43" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>389495930</v>
       </c>
@@ -1522,7 +1523,7 @@
         <v>62267</v>
       </c>
       <c r="F44" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1534,35 +1535,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3CA3B-7428-4B33-B0E2-6C158B81D988}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>21678</v>
@@ -1571,12 +1570,12 @@
         <v>43986.580555555556</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>73643</v>
@@ -1585,12 +1584,12 @@
         <v>44061.652777777781</v>
       </c>
       <c r="D3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
       </c>
       <c r="B4">
         <v>39493</v>
@@ -1599,12 +1598,12 @@
         <v>44185.167361111111</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>90384</v>
@@ -1613,12 +1612,12 @@
         <v>44196</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>23947</v>
@@ -1627,12 +1626,12 @@
         <v>43842</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>27429</v>
@@ -1641,12 +1640,12 @@
         <v>44127</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>42477</v>
@@ -1655,12 +1654,12 @@
         <v>44134</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>23394</v>
@@ -1669,12 +1668,12 @@
         <v>44156</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>29404</v>
@@ -1683,12 +1682,12 @@
         <v>44229</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>49249</v>
@@ -1697,12 +1696,12 @@
         <v>44307</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>94029</v>
@@ -1711,12 +1710,12 @@
         <v>44330</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>94944</v>
@@ -1725,12 +1724,12 @@
         <v>43633</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>93948</v>
@@ -1739,12 +1738,12 @@
         <v>43667</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B15">
         <v>23949</v>
@@ -1753,12 +1752,12 @@
         <v>43687</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>20420</v>
@@ -1767,12 +1766,12 @@
         <v>43851</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>85020</v>
@@ -1781,12 +1780,12 @@
         <v>43878</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>12739</v>
@@ -1795,12 +1794,12 @@
         <v>43585</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B19">
         <v>53432</v>
@@ -1809,12 +1808,12 @@
         <v>44177</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>28098</v>
@@ -1823,12 +1822,12 @@
         <v>44068</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>40478</v>
@@ -1837,12 +1836,12 @@
         <v>44151</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B22">
         <v>36170</v>
@@ -1851,12 +1850,12 @@
         <v>44312</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>83281</v>
@@ -1865,12 +1864,12 @@
         <v>43646</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B24">
         <v>39366</v>
@@ -1879,12 +1878,12 @@
         <v>44070</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>38129</v>
@@ -1893,12 +1892,12 @@
         <v>44087</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B26">
         <v>60489</v>
@@ -1907,12 +1906,12 @@
         <v>44188</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B27">
         <v>59410</v>
@@ -1921,12 +1920,12 @@
         <v>44181</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>60228</v>
@@ -1935,12 +1934,12 @@
         <v>43467</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B29">
         <v>74420</v>
@@ -1949,12 +1948,12 @@
         <v>43964</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B30">
         <v>30861</v>
@@ -1963,12 +1962,12 @@
         <v>43938</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B31">
         <v>49212</v>
@@ -1977,12 +1976,12 @@
         <v>43965</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B32">
         <v>59226</v>
@@ -1991,12 +1990,12 @@
         <v>44036</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B33">
         <v>27915</v>
@@ -2005,12 +2004,12 @@
         <v>44071</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B34">
         <v>66470</v>
@@ -2019,12 +2018,12 @@
         <v>44303</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B35">
         <v>54771</v>
@@ -2033,12 +2032,12 @@
         <v>44104</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B36">
         <v>33046</v>
@@ -2047,12 +2046,12 @@
         <v>43937</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="B37">
         <v>73447</v>
@@ -2061,12 +2060,12 @@
         <v>43468</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B38">
         <v>82199</v>
@@ -2075,12 +2074,12 @@
         <v>44211</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B39">
         <v>46278</v>
@@ -2089,12 +2088,12 @@
         <v>44253</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="B40">
         <v>76213</v>
@@ -2103,12 +2102,12 @@
         <v>44091</v>
       </c>
       <c r="D40" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B41">
         <v>28621</v>
@@ -2117,12 +2116,12 @@
         <v>43925</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B42">
         <v>59757</v>
@@ -2131,12 +2130,12 @@
         <v>43977</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="B43">
         <v>38699</v>
@@ -2145,12 +2144,12 @@
         <v>43990</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B44">
         <v>62267</v>
@@ -2159,7 +2158,7 @@
         <v>43914</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2172,265 +2171,265 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41668EC7-99C6-452E-83D6-A07D9880DEED}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2">
         <v>14310</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2">
         <v>19571</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C4" s="2">
         <v>15134</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C5" s="2">
         <v>15370</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2">
         <v>14322</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2">
         <v>17941</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2">
         <v>15759</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C9" s="2">
         <v>19898</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C10" s="2">
         <v>14823</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C11" s="2">
         <v>14322</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2">
         <v>13169</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C13" s="2">
         <v>14825</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C14" s="2">
         <v>19354</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2">
         <v>13899</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C16" s="2">
         <v>18990</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2">
         <v>18265</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2">
         <v>17573</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C19" s="2">
         <v>18540</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2">
         <v>19787</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2">
         <v>15943</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2">
         <v>15953</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>8547939598</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C23" s="1">
         <v>19821</v>

</xml_diff>